<commit_message>
No H-MYR-249 errors, and other new modifications
</commit_message>
<xml_diff>
--- a/milfoil_app/Herbicide_response_table.xlsx
+++ b/milfoil_app/Herbicide_response_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleywolfe/Documents/milfoil_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870C59BC-EF85-F943-A491-963D5DE0E06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2467FE-7C38-AD4B-9806-79BDC070162B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{0D5F135C-3651-DD43-AA6C-7580DD447B7D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{0D5F135C-3651-DD43-AA6C-7580DD447B7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Microsat_ID</t>
   </si>
@@ -59,12 +59,6 @@
     <t>H_MISGP_231</t>
   </si>
   <si>
-    <t>Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.</t>
-  </si>
-  <si>
-    <t>Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.</t>
-  </si>
-  <si>
     <t>H_MISGP_187</t>
   </si>
   <si>
@@ -89,22 +83,164 @@
     <t>H_MYR_7905</t>
   </si>
   <si>
-    <t>H_MYR_1799</t>
-  </si>
-  <si>
     <t>H_MYR_11345</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Herbicide assays performed in the Thum lab for this strain, have shown this strain is fluridone resistant and does not respond well when treated with fluridone. We recommend not using fluridone if this strain is present in your lake. Please see Chorak and Thum 2020, and Berger et al 2012.</t>
-  </si>
-  <si>
-    <t>Herbicide assays performed in the Thum lab for this strain, have shown this strain is fluridone resistant and does not respond well when treated with fluridone. We recommend not using fluridone if this strain is present in your lake. Please see Chorak and Thum 2020, and Berger et al. 2012.</t>
-  </si>
-  <si>
-    <t>Herbicide assays performed in the Thum lab for this strain, show the strain to be resistant to 2,4-D. We recommend not using 2,4-D if this strain is present in your lake. When available, please see Hoff et al. in revision.</t>
+    <t>E_MISGP_1863</t>
+  </si>
+  <si>
+    <t>H_MISGP_1799</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = E_MISGP_1802&gt;E_MISGP_1802&lt;/h3&gt;&lt;/P&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = E_MISGP_1802&gt;E_MISGP_1802&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = E_MISGP_380&gt;E_MISGP_380&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;h2&gt;
+&lt;p&gt;&lt;h3 id = E_MISGP_380&gt;E_MISGP_380&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, have shown this strain is fluridone resistant and does not respond well when treated with fluridone. We recommend not using fluridone if this strain is present in your lake. Please see &lt;a href = 'https://doi.org/10.1017/inp.2020.34'&gt;Chorak and Thum 2020.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = E_MISGP_734&gt;E_MISGP_734&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = E_MISGP_734&gt;E_MISGP_734&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_187&gt;H_MISGP_187&lt;/h3&gt;&lt;p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_187&gt;H_MISGP_187&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_249&gt;H_MISGP_249&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, have shown this strain is fluridone resistant and does not respond well when treated with fluridone. We recommend not using fluridone if this strain is present in your lake. Please see &lt;a href = 'https://doi.org/10.1017/inp.2020.34'&gt;Chorak and Thum 2020 &lt;/a&gt; and &lt;a href = 'https://doi.org/10.1614/WS-D-14-00085.1'&gt;Berger et al. 2012&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_249&gt;H_MISGP_249&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_464&gt;H_MISGP_464&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_464&gt;H_MISGP_464&lt;/h3&gt;&lt;/P&gt;
+&lt;p&gt;At this time, the 2,4-D herbicide response for this strain is unknown.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_518&gt;H_MISGP_518&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_518&gt;H_MISGP_518&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MYR_10199&gt;H_MYR_10199&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MYR_10199&gt;H_MYR_10199&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MYR_4866&gt;H_MYR_4866&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MYR_4866&gt;H_MYR_4866&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MYR_5016&gt;H_MYR_5016&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MYR_5016&gt;H_MYR_5016&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be resistant to 2,4-D. We recommend not using 2,4-D if this strain is present in your lake. Hoff et al. unpublished data.&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MYR_7905&gt;H_MYR_7905&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;At this time, the 2,4-D herbicide response for this strain is unknown.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MYR_7905&gt;H_MYR_7905&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;&lt;h3&gt;H_MYR_7905&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MYR_11345&gt;H_MYR_11345&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MYR_11345&gt;H_MYR_11345&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;At this time, the 2,4-D herbicide response for this strain is unknown.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = E_MISGP_1863&gt;E_MISGP_1863&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = E_MISGP_1863&gt;E_MISGP_1863&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_1799&gt;H_MISGP_1799&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_1799&gt;H_MISGP_1799&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;2,4-D Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_231&gt;H_MISGP_231&lt;/h3&gt;&lt;p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to 2,4-D. However, it is always good to continue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Fluridone Response&lt;/h2&gt;
+&lt;p&gt;&lt;h3 id = H_MISGP_231&gt;H_MISGP_231&lt;/h3&gt;&lt;/p&gt;
+&lt;p&gt;Herbicide assays performed in the Thum lab for this strain, show the strain to be sensitive in response to fluridone. However, it is always good to conintue to monitor the efficacy of treatment in your lake.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -473,18 +609,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A656422D-075E-D341-ABA8-E8A10BAE04A2}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="36.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39" style="1" customWidth="1"/>
+    <col min="4" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="82" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -498,18 +636,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="221" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="153" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="238" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="204" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -517,139 +655,150 @@
         <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="153" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="238" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="170" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="170" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="238" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="170" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="170" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="170" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="170" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="187" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="170" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="170" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="170" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>